<commit_message>
Se agrega lista de excluidos en excel
</commit_message>
<xml_diff>
--- a/Reporte Mids - 18-02-2024.xlsx
+++ b/Reporte Mids - 18-02-2024.xlsx
@@ -67,25 +67,22 @@
     <col min="4" max="4" width="19.7890625" customWidth="true"/>
     <col min="5" max="5" width="21.59765625" customWidth="true"/>
     <col min="6" max="6" width="48.3828125" customWidth="true"/>
-    <col min="7" max="7" width="7.7734375" customWidth="true"/>
+    <col min="7" max="7" width="17.89453125" customWidth="true"/>
     <col min="8" max="8" width="17.89453125" customWidth="true"/>
-    <col min="9" max="9" width="17.89453125" customWidth="true"/>
-    <col min="10" max="10" width="8.05078125" customWidth="true"/>
-    <col min="11" max="11" width="15.87890625" customWidth="true"/>
-    <col min="12" max="12" width="34.23046875" customWidth="true"/>
-    <col min="13" max="13" width="15.34375" customWidth="true"/>
-    <col min="14" max="14" width="12.2578125" customWidth="true"/>
-    <col min="15" max="15" width="12.0625" customWidth="true"/>
-    <col min="16" max="16" width="28.484375" customWidth="true"/>
-    <col min="17" max="17" width="5.38671875" customWidth="true"/>
-    <col min="18" max="18" width="9.87890625" customWidth="true"/>
-    <col min="19" max="19" width="9.16796875" customWidth="true"/>
-    <col min="20" max="20" width="30.34765625" customWidth="true"/>
-    <col min="21" max="21" width="19.37109375" customWidth="true"/>
-    <col min="22" max="22" width="17.5390625" customWidth="true"/>
-    <col min="23" max="23" width="9.68359375" customWidth="true"/>
-    <col min="24" max="24" width="10.5078125" customWidth="true"/>
-    <col min="25" max="25" width="29.578125" customWidth="true"/>
+    <col min="9" max="9" width="8.05078125" customWidth="true"/>
+    <col min="10" max="10" width="15.87890625" customWidth="true"/>
+    <col min="11" max="11" width="34.23046875" customWidth="true"/>
+    <col min="12" max="12" width="15.34375" customWidth="true"/>
+    <col min="13" max="13" width="12.2578125" customWidth="true"/>
+    <col min="14" max="14" width="12.0625" customWidth="true"/>
+    <col min="15" max="15" width="28.484375" customWidth="true"/>
+    <col min="16" max="16" width="5.38671875" customWidth="true"/>
+    <col min="17" max="17" width="9.87890625" customWidth="true"/>
+    <col min="18" max="18" width="30.34765625" customWidth="true"/>
+    <col min="19" max="19" width="19.37109375" customWidth="true"/>
+    <col min="20" max="20" width="17.5390625" customWidth="true"/>
+    <col min="21" max="21" width="9.68359375" customWidth="true"/>
+    <col min="22" max="22" width="10.5078125" customWidth="true"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -121,97 +118,82 @@
       </c>
       <c r="G1" t="inlineStr">
         <is>
-          <t>ACTIVO</t>
+          <t>ADQVISA</t>
         </is>
       </c>
       <c r="H1" t="inlineStr">
         <is>
-          <t>ADQVISA</t>
+          <t>ADQVSD</t>
         </is>
       </c>
       <c r="I1" t="inlineStr">
         <is>
-          <t>ADQVSD</t>
+          <t>CIUDAD</t>
         </is>
       </c>
       <c r="J1" t="inlineStr">
         <is>
-          <t>CIUDAD</t>
+          <t>COMUNICACION</t>
         </is>
       </c>
       <c r="K1" t="inlineStr">
         <is>
-          <t>COMUNICACION</t>
+          <t>DIRECCION</t>
         </is>
       </c>
       <c r="L1" t="inlineStr">
         <is>
-          <t>DIRECCION</t>
+          <t>RUC</t>
         </is>
       </c>
       <c r="M1" t="inlineStr">
         <is>
-          <t>RUC</t>
+          <t>DISPOSITIVO</t>
         </is>
       </c>
       <c r="N1" t="inlineStr">
         <is>
-          <t>DISPOSITIVO</t>
+          <t>MID</t>
         </is>
       </c>
       <c r="O1" t="inlineStr">
         <is>
-          <t>MID</t>
+          <t>GIRO_NEGOCIO</t>
         </is>
       </c>
       <c r="P1" t="inlineStr">
         <is>
-          <t>GIRO_NEGOCIO</t>
+          <t>MCC</t>
         </is>
       </c>
       <c r="Q1" t="inlineStr">
         <is>
-          <t>MCC</t>
+          <t>TID</t>
         </is>
       </c>
       <c r="R1" t="inlineStr">
         <is>
-          <t>TID</t>
+          <t>ADQMCD</t>
         </is>
       </c>
       <c r="S1" t="inlineStr">
         <is>
-          <t>USUARIO</t>
+          <t>FECHA_ASIGNACION</t>
         </is>
       </c>
       <c r="T1" t="inlineStr">
         <is>
-          <t>ADQMCD</t>
+          <t>COD_BCO_DINERS</t>
         </is>
       </c>
       <c r="U1" t="inlineStr">
         <is>
-          <t>FECHA_ASIGNACION</t>
+          <t>MODELO</t>
         </is>
       </c>
       <c r="V1" t="inlineStr">
         <is>
-          <t>COD_BCO_DINERS</t>
-        </is>
-      </c>
-      <c r="W1" t="inlineStr">
-        <is>
-          <t>MODELO</t>
-        </is>
-      </c>
-      <c r="X1" t="inlineStr">
-        <is>
           <t>TELEFONO</t>
-        </is>
-      </c>
-      <c r="Y1" t="inlineStr">
-        <is>
-          <t>FECHA_ACTUAL</t>
         </is>
       </c>
     </row>
@@ -248,7 +230,7 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>ACT</t>
+          <t>BANCO PICHINCHA</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
@@ -258,87 +240,72 @@
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>BANCO PICHINCHA</t>
+          <t>QUITO</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>QUITO</t>
+          <t>DIAL</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>DIAL</t>
+          <t>VIA INTEREOCEANICA SN Y G SUAREZ</t>
         </is>
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>VIA INTEREOCEANICA SN Y G SUAREZ</t>
+          <t>1790016919001</t>
         </is>
       </c>
       <c r="M2" t="inlineStr">
         <is>
-          <t>1790016919001</t>
+          <t>C</t>
         </is>
       </c>
       <c r="N2" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>2000001121</t>
         </is>
       </c>
       <c r="O2" t="inlineStr">
         <is>
-          <t>2000001121</t>
+          <t>ABARROTES SUPERMERCADOS</t>
         </is>
       </c>
       <c r="P2" t="inlineStr">
         <is>
-          <t>ABARROTES SUPERMERCADOS</t>
+          <t>5411</t>
         </is>
       </c>
       <c r="Q2" t="inlineStr">
         <is>
-          <t>5411</t>
+          <t>00112001</t>
         </is>
       </c>
       <c r="R2" t="inlineStr">
         <is>
-          <t>00112001</t>
+          <t>BANCO GUAYAQUIL  PACIFICARD</t>
         </is>
       </c>
       <c r="S2" t="inlineStr">
         <is>
-          <t>JMUNOZ</t>
+          <t>2000-01-01</t>
         </is>
       </c>
       <c r="T2" t="inlineStr">
         <is>
-          <t>BANCO GUAYAQUIL  PACIFICARD</t>
+          <t>532508</t>
         </is>
       </c>
       <c r="U2" t="inlineStr">
         <is>
-          <t>2000-01-01</t>
+          <t>CAJA-REG</t>
         </is>
       </c>
       <c r="V2" t="inlineStr">
         <is>
-          <t>532508</t>
-        </is>
-      </c>
-      <c r="W2" t="inlineStr">
-        <is>
-          <t>CAJA-REG</t>
-        </is>
-      </c>
-      <c r="X2" t="inlineStr">
-        <is>
           <t/>
-        </is>
-      </c>
-      <c r="Y2" t="inlineStr">
-        <is>
-          <t>2024-02-17T21:22:15.333+0000</t>
         </is>
       </c>
     </row>
@@ -375,7 +342,7 @@
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>ACT</t>
+          <t>BANCO PICHINCHA</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
@@ -385,87 +352,72 @@
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>BANCO PICHINCHA</t>
+          <t>QUITO</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>QUITO</t>
+          <t>DIAL</t>
         </is>
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>DIAL</t>
+          <t>VIA INTEREOCEANICA SN Y G SUAREZ</t>
         </is>
       </c>
       <c r="L3" t="inlineStr">
         <is>
-          <t>VIA INTEREOCEANICA SN Y G SUAREZ</t>
+          <t>1790016919001</t>
         </is>
       </c>
       <c r="M3" t="inlineStr">
         <is>
-          <t>1790016919001</t>
+          <t>C</t>
         </is>
       </c>
       <c r="N3" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>2000001121</t>
         </is>
       </c>
       <c r="O3" t="inlineStr">
         <is>
-          <t>2000001121</t>
+          <t>ABARROTES SUPERMERCADOS</t>
         </is>
       </c>
       <c r="P3" t="inlineStr">
         <is>
-          <t>ABARROTES SUPERMERCADOS</t>
+          <t>5411</t>
         </is>
       </c>
       <c r="Q3" t="inlineStr">
         <is>
-          <t>5411</t>
+          <t>00112002</t>
         </is>
       </c>
       <c r="R3" t="inlineStr">
         <is>
-          <t>00112002</t>
+          <t>BANCO GUAYAQUIL  PACIFICARD</t>
         </is>
       </c>
       <c r="S3" t="inlineStr">
         <is>
-          <t>JMUNOZ</t>
+          <t>2000-01-01</t>
         </is>
       </c>
       <c r="T3" t="inlineStr">
         <is>
-          <t>BANCO GUAYAQUIL  PACIFICARD</t>
+          <t>532508</t>
         </is>
       </c>
       <c r="U3" t="inlineStr">
         <is>
-          <t>2000-01-01</t>
+          <t>CAJA-REG</t>
         </is>
       </c>
       <c r="V3" t="inlineStr">
         <is>
-          <t>532508</t>
-        </is>
-      </c>
-      <c r="W3" t="inlineStr">
-        <is>
-          <t>CAJA-REG</t>
-        </is>
-      </c>
-      <c r="X3" t="inlineStr">
-        <is>
           <t/>
-        </is>
-      </c>
-      <c r="Y3" t="inlineStr">
-        <is>
-          <t>2024-02-17T21:22:15.333+0000</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Se agrega excel con multiples hojas
</commit_message>
<xml_diff>
--- a/Reporte Mids - 18-02-2024.xlsx
+++ b/Reporte Mids - 18-02-2024.xlsx
@@ -6,7 +6,8 @@
     <workbookView activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Datos" r:id="rId3" sheetId="1"/>
+    <sheet name="caja" r:id="rId3" sheetId="1"/>
+    <sheet name="post" r:id="rId4" sheetId="2"/>
   </sheets>
 </workbook>
 </file>
@@ -424,4 +425,377 @@
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <cols>
+    <col min="1" max="1" width="8.48046875" customWidth="true"/>
+    <col min="2" max="2" width="17.20703125" customWidth="true"/>
+    <col min="3" max="3" width="7.64453125" customWidth="true"/>
+    <col min="4" max="4" width="19.7890625" customWidth="true"/>
+    <col min="5" max="5" width="21.59765625" customWidth="true"/>
+    <col min="6" max="6" width="48.3828125" customWidth="true"/>
+    <col min="7" max="7" width="17.89453125" customWidth="true"/>
+    <col min="8" max="8" width="17.89453125" customWidth="true"/>
+    <col min="9" max="9" width="8.05078125" customWidth="true"/>
+    <col min="10" max="10" width="15.87890625" customWidth="true"/>
+    <col min="11" max="11" width="34.23046875" customWidth="true"/>
+    <col min="12" max="12" width="15.34375" customWidth="true"/>
+    <col min="13" max="13" width="12.2578125" customWidth="true"/>
+    <col min="14" max="14" width="12.0625" customWidth="true"/>
+    <col min="15" max="15" width="28.484375" customWidth="true"/>
+    <col min="16" max="16" width="5.38671875" customWidth="true"/>
+    <col min="17" max="17" width="9.87890625" customWidth="true"/>
+    <col min="18" max="18" width="30.34765625" customWidth="true"/>
+    <col min="19" max="19" width="19.37109375" customWidth="true"/>
+    <col min="20" max="20" width="17.5390625" customWidth="true"/>
+    <col min="21" max="21" width="9.68359375" customWidth="true"/>
+    <col min="22" max="22" width="10.5078125" customWidth="true"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>CORREO</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>POLITICA_EQUIPO</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>MARCA</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>INTEROPERABILIDAD</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>COMERCIO</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>ADQMC</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>ADQVISA</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>ADQVSD</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>CIUDAD</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>COMUNICACION</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>DIRECCION</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>RUC</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>DISPOSITIVO</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>MID</t>
+        </is>
+      </c>
+      <c r="O1" t="inlineStr">
+        <is>
+          <t>GIRO_NEGOCIO</t>
+        </is>
+      </c>
+      <c r="P1" t="inlineStr">
+        <is>
+          <t>MCC</t>
+        </is>
+      </c>
+      <c r="Q1" t="inlineStr">
+        <is>
+          <t>TID</t>
+        </is>
+      </c>
+      <c r="R1" t="inlineStr">
+        <is>
+          <t>ADQMCD</t>
+        </is>
+      </c>
+      <c r="S1" t="inlineStr">
+        <is>
+          <t>FECHA_ASIGNACION</t>
+        </is>
+      </c>
+      <c r="T1" t="inlineStr">
+        <is>
+          <t>COD_BCO_DINERS</t>
+        </is>
+      </c>
+      <c r="U1" t="inlineStr">
+        <is>
+          <t>MODELO</t>
+        </is>
+      </c>
+      <c r="V1" t="inlineStr">
+        <is>
+          <t>TELEFONO</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>V</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">   </t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>AUSTRO - MEDIANET</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>SUPERMAXI TUMBACO</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>BANCO GUAYAQUIL  BANCO PICHINCHA  PACIFICARD</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>BANCO PICHINCHA</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>BANCO PICHINCHA</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>QUITO</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>DIAL</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>VIA INTEREOCEANICA SN Y G SUAREZ</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>1790016919001</t>
+        </is>
+      </c>
+      <c r="M2" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="N2" t="inlineStr">
+        <is>
+          <t>2000001121</t>
+        </is>
+      </c>
+      <c r="O2" t="inlineStr">
+        <is>
+          <t>ABARROTES SUPERMERCADOS</t>
+        </is>
+      </c>
+      <c r="P2" t="inlineStr">
+        <is>
+          <t>5411</t>
+        </is>
+      </c>
+      <c r="Q2" t="inlineStr">
+        <is>
+          <t>00112001</t>
+        </is>
+      </c>
+      <c r="R2" t="inlineStr">
+        <is>
+          <t>BANCO GUAYAQUIL  PACIFICARD</t>
+        </is>
+      </c>
+      <c r="S2" t="inlineStr">
+        <is>
+          <t>2000-01-01</t>
+        </is>
+      </c>
+      <c r="T2" t="inlineStr">
+        <is>
+          <t>532508</t>
+        </is>
+      </c>
+      <c r="U2" t="inlineStr">
+        <is>
+          <t>CAJA-REG</t>
+        </is>
+      </c>
+      <c r="V2" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>V</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">   </t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>AUSTRO - MEDIANET</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>SUPERMAXI TUMBACO</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>BANCO GUAYAQUIL  BANCO PICHINCHA  PACIFICARD</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>BANCO PICHINCHA</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>BANCO PICHINCHA</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>QUITO</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>DIAL</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>VIA INTEREOCEANICA SN Y G SUAREZ</t>
+        </is>
+      </c>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>1790016919001</t>
+        </is>
+      </c>
+      <c r="M3" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="N3" t="inlineStr">
+        <is>
+          <t>2000001121</t>
+        </is>
+      </c>
+      <c r="O3" t="inlineStr">
+        <is>
+          <t>ABARROTES SUPERMERCADOS</t>
+        </is>
+      </c>
+      <c r="P3" t="inlineStr">
+        <is>
+          <t>5411</t>
+        </is>
+      </c>
+      <c r="Q3" t="inlineStr">
+        <is>
+          <t>00112002</t>
+        </is>
+      </c>
+      <c r="R3" t="inlineStr">
+        <is>
+          <t>BANCO GUAYAQUIL  PACIFICARD</t>
+        </is>
+      </c>
+      <c r="S3" t="inlineStr">
+        <is>
+          <t>2000-01-01</t>
+        </is>
+      </c>
+      <c r="T3" t="inlineStr">
+        <is>
+          <t>532508</t>
+        </is>
+      </c>
+      <c r="U3" t="inlineStr">
+        <is>
+          <t>CAJA-REG</t>
+        </is>
+      </c>
+      <c r="V3" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
 </file>
</xml_diff>